<commit_message>
update(index.js): result-file has name as input-file
</commit_message>
<xml_diff>
--- a/src/xlsx/template.xlsx
+++ b/src/xlsx/template.xlsx
@@ -19,13 +19,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Key</t>
+    <t>Ключ</t>
   </si>
   <si>
-    <t>Initial value</t>
+    <t>Значение на русском</t>
   </si>
   <si>
-    <t>New Value</t>
+    <t>Значение на казахском</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>